<commit_message>
[ADD] Vendor Service CSV added
</commit_message>
<xml_diff>
--- a/mtbl_installer/data_defination/MTB_DATA MAPPING__Vendorr.xlsx
+++ b/mtbl_installer/data_defination/MTB_DATA MAPPING__Vendorr.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="VENDOR_DATA" sheetId="1" state="visible" r:id="rId2"/>
@@ -134,7 +134,7 @@
     <t xml:space="preserve">info@tkgroupbd.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Shah Ali</t>
+    <t xml:space="preserve">Tejgaon</t>
   </si>
   <si>
     <t xml:space="preserve">Manager</t>
@@ -270,14 +270,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
-    <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -336,11 +335,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -409,7 +403,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -470,10 +464,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -482,7 +472,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -490,15 +480,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -521,39 +507,38 @@
   </sheetPr>
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V2" activeCellId="0" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -829,16 +814,19 @@
   </sheetPr>
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="1" sqref="3:3 B30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="21.9489795918367"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="17.5051020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -921,24 +909,25 @@
       <c r="A4" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="17" t="s">
+      <c r="E4" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>63</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="H4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="n">
@@ -950,18 +939,19 @@
       <c r="C5" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="17" t="s">
+      <c r="D5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="H5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="n">
@@ -973,18 +963,19 @@
       <c r="C6" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="17" t="s">
+      <c r="D6" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="H6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="n">
@@ -996,13 +987,13 @@
       <c r="C7" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="17" t="s">
+      <c r="E7" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G7" s="6" t="s">
@@ -1022,18 +1013,19 @@
       <c r="C8" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="18" t="s">
+      <c r="D8" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G8" s="6" t="n">
         <v>1234567891234560</v>
       </c>
+      <c r="H8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="n">
@@ -1045,18 +1037,19 @@
       <c r="C9" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="D9" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>31</v>
       </c>
+      <c r="H9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="n">
@@ -1068,18 +1061,19 @@
       <c r="C10" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="17" t="s">
+      <c r="D10" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>63</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="H10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="n">
@@ -1091,18 +1085,19 @@
       <c r="C11" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="17" t="s">
+      <c r="D11" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="H11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="n">
@@ -1114,13 +1109,13 @@
       <c r="C12" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="17" t="s">
+      <c r="D12" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -1140,18 +1135,19 @@
       <c r="C13" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="17" t="s">
+      <c r="D13" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="H13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="n">
@@ -1163,18 +1159,19 @@
       <c r="C14" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="17" t="s">
+      <c r="D14" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G14" s="6" t="n">
         <v>9114332</v>
       </c>
+      <c r="H14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="14" t="n">
@@ -1186,18 +1183,19 @@
       <c r="C15" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="17" t="s">
+      <c r="D15" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G15" s="6" t="n">
         <v>19144136</v>
       </c>
+      <c r="H15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="n">
@@ -1209,18 +1207,19 @@
       <c r="C16" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G16" s="19" t="n">
+      <c r="D16" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="18" t="n">
         <v>9142333391423330</v>
       </c>
+      <c r="H16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="n">
@@ -1232,18 +1231,19 @@
       <c r="C17" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="17" t="s">
+      <c r="D17" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>36</v>
       </c>
+      <c r="H17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="n">
@@ -1255,18 +1255,19 @@
       <c r="C18" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="18" t="s">
+      <c r="D18" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G18" s="6" t="n">
         <v>417149</v>
       </c>
+      <c r="H18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="n">
@@ -1278,18 +1279,19 @@
       <c r="C19" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="18" t="s">
+      <c r="D19" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="17" t="n">
+      <c r="F19" s="16" t="n">
         <v>11</v>
       </c>
       <c r="G19" s="6" t="n">
         <v>32156498712</v>
       </c>
+      <c r="H19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="n">
@@ -1301,18 +1303,19 @@
       <c r="C20" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="18" t="s">
+      <c r="D20" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="17" t="n">
+      <c r="F20" s="16" t="n">
         <v>9</v>
       </c>
       <c r="G20" s="6" t="n">
         <v>989811122</v>
       </c>
+      <c r="H20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="n">
@@ -1324,18 +1327,19 @@
       <c r="C21" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="18" t="s">
+      <c r="D21" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="17" t="n">
+      <c r="F21" s="16" t="n">
         <v>12</v>
       </c>
       <c r="G21" s="6" t="n">
         <v>646897646998</v>
       </c>
+      <c r="H21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="n">
@@ -1347,18 +1351,19 @@
       <c r="C22" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="18" t="s">
+      <c r="D22" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="16" t="s">
         <v>73</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>9874573215</v>
       </c>
+      <c r="H22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="n">
@@ -1370,18 +1375,19 @@
       <c r="C23" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" s="17" t="s">
+      <c r="D23" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="H23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="n">
@@ -1393,18 +1399,19 @@
       <c r="C24" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F24" s="17" t="s">
+      <c r="D24" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="H24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="n">
@@ -1416,18 +1423,19 @@
       <c r="C25" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" s="17" t="s">
+      <c r="D25" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="H25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="n">
@@ -1439,18 +1447,19 @@
       <c r="C26" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="17" t="s">
+      <c r="D26" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G26" s="6" t="n">
         <v>1216</v>
       </c>
+      <c r="H26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="14" t="n">
@@ -1462,18 +1471,19 @@
       <c r="C27" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="17" t="s">
+      <c r="D27" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="H27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="14" t="n">
@@ -1485,19 +1495,20 @@
       <c r="C28" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G28" s="20" t="b">
+      <c r="D28" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="19" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H28" s="21" t="n">
+      <c r="H28" s="20" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1512,19 +1523,20 @@
       <c r="C29" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" s="20" t="b">
+      <c r="D29" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="19" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H29" s="22" t="n">
+      <c r="H29" s="19" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1539,13 +1551,13 @@
       <c r="C30" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="17" t="s">
+      <c r="D30" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G30" s="6" t="s">

</xml_diff>